<commit_message>
add grades in both csvs and display correct courses+grades the student has taken
</commit_message>
<xml_diff>
--- a/CS Student.xlsx
+++ b/CS Student.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuantang/Desktop/sms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuantang/Desktop/Student-Course-Recommendation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B29B4-400B-6243-B3A3-758D397D0ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A1379C-4A1D-D942-B31E-45E8C39950A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="28240" windowHeight="17440" xr2:uid="{1B581FCD-855C-764C-99A5-299B417155D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,121 +59,57 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;HIS104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Bryson</t>
   </si>
   <si>
-    <t>CS112;CS122;CS151;MATH122;MATH241;ENG101;PSY102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sawyer</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;HIS104;PSY102;CHEM105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Jason</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS281;CS440;CS455;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ECE100;PSY102;CHEM105;PHILOS100;ENG270;HIS104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cole</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;PHY141;CHEM105;ENG101;PSY102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Luis</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS281;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;HIS104;PSY102;CHEM105;PHILOS100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Calvin</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;ENG101;CHEM105;PSY102;ECE100;PHY141;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Zion</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS455;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;BUSI100;PSY102;CHEM105;PSY211</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Carlos</t>
   </si>
   <si>
-    <t>CS112;CS122;CS151;MATH122;MATH241;ENG101;CHEM105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Lorenzo</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS281;CS462;MATH122;MATH241;MATH259;ENG101;PHY141;ECE100;HIS104;PSY102;CHEM105;PSY211</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Elliott</t>
   </si>
   <si>
-    <t>CS112;CS122;CS151;MATH122;MATH241;ENG101;PHY141</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Karter</t>
   </si>
   <si>
-    <t>CS112;CS122;CS151;MATH122;MATH241;ENG101;BIO121</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Thiago</t>
   </si>
   <si>
     <t>Brandon</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS281;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ENG270;PSY102;CHEM105;PHILOS100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Justin</t>
   </si>
   <si>
     <t>Matteo</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ECE100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Hayden</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;ENG101;ECO102;PHY141;CHEM105;PSY102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Antonio</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;ENG101;PHY141;HIS104;CHEM105;ENG270;BIO121</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Abel</t>
   </si>
   <si>
@@ -184,197 +120,289 @@
     <t>Tristan</t>
   </si>
   <si>
-    <t>CS112;MATH122</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Zayden</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS440;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ENG270;PSY102;BIO121;PHILOS100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Miguel</t>
   </si>
   <si>
     <t>Messiah</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;CHEM105;ECE100;ENG101;PSY102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tucker</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;ENG101;PSY102;PHY141;CHEM105;HIS104;BIO121</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Alan</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;CHEM105;PHY141;HIS104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Edward</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;CHEM105;PHY141;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Leon</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS440;ML315;CS462;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ENG270;PSY102;BIO121;PHILOS100;ECE100;PSY211</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Eric</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS330;CS440;CS455;HCI391;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ENG270;PSY102;BIO121;PHILOS100;CHEM105;BUSI100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ace</t>
   </si>
   <si>
     <t>Nicolas</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;ENG101;CHEM105;PSY102;HIS104;PHY141;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Charlie</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;BIO121;PHY141;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Blake</t>
   </si>
   <si>
-    <t>MATH122</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Avery</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;ENG101;ENG270;PSY102;HIS104;CHEM105;BIO121</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Colt</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;PHY141;HIS104;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Jaxon</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;HIS104;PSY102;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Josiah</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS462;CS281;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ENG270;PSY102;CHEM105;PHILOS100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Isaiah</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS330;CS281;CS440;ML315;MATH122;MATH241;MATH259;ENG101;PHY141;ECO102;ENG270;PSY102;CHEM105;PHILOS100;BIO121;PSY211</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Elias</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;BIO121;PHY141;ENG101;ECO102;ENG270;CHEM105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Joshua</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS330;CS317;CS440;CS281;MATH122;MATH241;MATH259;ENG101;ECE100;ECO102;ENG270;PSY102;CHEM105;BUSI100;BIO121;PSY211</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ryan</t>
   </si>
   <si>
     <t>Eli</t>
   </si>
   <si>
-    <t>CS112;CS122;CS151;MATH122;MATH259;ENG101;CHEM105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Nolan</t>
   </si>
   <si>
     <t>Ezekiel</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS330;CS281;MATH122;MATH241;MATH259;ENG101;PHY141;CHEM105;ENG270;PSY102;BUSI100;PHILOS100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Rafael</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;MATH122;MATH241;MATH259;BIO121;HIS104;ENG101;ECO102;ECE100;PSY141</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Maximus</t>
   </si>
   <si>
     <t>Theodore</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS281;CS330;HCI391;MATH122;MATH241;MATH259;ENG101;PHY141;HIS104;ENG270;PSY102;CHEM105;PHILOS100;BIO121;PSY211;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Samuel</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;MATH122;MATH241;MATH259;ENG101;CHEM105;BIO121;ECO102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>David</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS281;CS462;SWE214;ML315;MATH122;MATH241;MATH259;ENG101;PHY141;ECE100;ENG270;PSY102;CHEM105;PHILOS100;BIO121;HIS104;PSY211</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Wyatt</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS281;CS462;CS330;SWE214;MATH122;MATH241;MATH259;ENG101;PHY141;ECE100;ENG270;PSY102;CHEM105;PHILOS100;BIO121;HIS104;BUSI100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Luke</t>
   </si>
   <si>
-    <t>CS112;CS122;CS150;CS151;CS251;CS213;CS210;CS259;CS451;CS317;CS281;MATH122;MATH241;MATH259;ENG101;PHY141;ECE100;HIS104;PSY102;PSY211;PHILOS100</t>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:A;HIS104:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS151:A;MATH122:A;MATH241:A;ENG101:A;PSY102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:A;CS213:A;CS210:A;CS259:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:A;HIS104:C;PSY102:A;CHEM105:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:D;CS151:A;CS251:B;MATH122:A;MATH241:A;MATH259:A;PHY141:A;CHEM105:A;ENG101:A;PSY102:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:A;CS251:B;CS213:A;CS210:B;CS259:C;CS451:C;CS317:B;CS281:A;MATH122:B;MATH241:B;MATH259:B;ENG101:A;PHY141:A;ECO102:A;HIS104:B;PSY102:A;CHEM105:A;PHILOS100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:A;CS251:C;CS213:A;CS210:D;CS259:C;MATH122:A;MATH241:A;MATH259:A;ENG101:A;CHEM105:A;PSY102:A;ECE100:B;PHY141:A;ECO102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:A;CS21:3:A;CS210:A;CS259:A;CS451:A;CS317:A;CS455:A;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:A;BUSI100:A;PSY102:A;CHEM105:A;PSY211:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:D;CS151:B;MATH122:A;MATH241:A;ENG101:A;CHEM105:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:B;CS251:C;CS213:B;CS210:C;CS259:D;CS451:D;CS281:B;CS462:B;MATH122:A;MATH241:A;MATH259:A;ENG101:B;PHY141:A;ECE100:A;HIS104:B;PSY102:A;CHEM105:A;PSY211:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS151:B;MATH122:A;MATH241:B;ENG101:A;PHY141:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS151:A;MATH122:A;MATH241:A;ENG101:C;BIO121:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:B;CS122:A;CS150:C;CS151:B;CS251:C;CS213:D;CS210:B;CS259:C;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:A;HIS104:A;PSY102:B;CHEM105:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:A;CS213:A;CS210:B;CS259:B;CS451:B;CS317:D;CS281:A;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:A;ENG270:B;PSY102:B;CHEM105:A;PHILOS100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS151:A;MATH122:A;MATH241:A;ENG101:A;BIO121:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:B;CS122:B;CS150:D;CS151:B;CS251:D;MATH122:A;MATH241:B;MATH259:B;ENG101:A;PHY141:A;ECO102:A;ECE100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:A;CS251:B;CS213:A;CS210:C;CS259:C;MATH122:A;MATH241:B;MATH259:A;ENG101:A;ECO102:A;PHY141:A;CHEM105:A;PSY102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:B;CS213:A;CS210:A;CS259:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;HIS104:B;CHEM105:A;ENG270:A;BIO121:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;MATH122:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:A;CS151:A;CS251:B;CS213:A;CS210:B;CS259:C;CS451:C;CS317:B;CS440:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:A;ENG270:A;PSY102:A;BIO121:A;PHILOS100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:D;CS151:D;MATH122:B;MATH241:A;ENG101:B;BIO121:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:C;CS251:D;MATH122:A;MATH241:D;MATH259:B;CHEM105:A;ECE100:A;ENG101:E;PSY102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:A;CS213:D;CS210:A;CS259:B;MATH122:A;MATH241;A;MATH259:A;ENG101:A;PSY102:A;PHY141:A;CHEM105:B;HIS104:A;BIO121:C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:B;CS251:B;MATH122:A;MATH241:D;MATH259:B;ENG101:D;CHEM105:A;PHY141:B;HIS104:D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:A;MATH122:A;MATH241:A;MATH259:A;ENG101:A;CHEM105:A;PHY141:A;ECO102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:A;CS213:A;CS210:B;CS259:C;CS451:D;CS317:B;CS440:D;ML315:B;CS462:C;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:B;ECO102:A;ENG270:A;PSY102:A;BIO121:A;PHILOS100:A;ECE100:A;PSY211:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:B;CS122:A;CS150:B;CS151:A;CS251:B;CS213:B;CS210:B;CS259:C;CS451:B;CS330:C;CS440:B;CS455:C;HCI391:A;MATH122:A;MATH241:B;MATH259:C;ENG101:A;PHY141:A;ECO102:B;ENG270:B;PSY102:A;BIO121:B;PHILOS100:A;CHEM105:A;BUSI100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:B;CS151:C;CS251:A;CS213:A;CS210:D;CS259:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PSY102:A;PHY141:A;CHEM105:A;HIS104:B;BIO121:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:A;CS151:B;CS251:C;CS213:D;CS210:B;CS259:B;MATH122:A;MATH241:A;MATH259:A;ENG101:D;CHEM105:A;PSY102:A;HIS104:D;PHY141:A;ECO102:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MATH122:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:D;MATH122:B;MATH241:D;MATH259:B;ENG101:B;BIO121:A;PHY141:A;ECO102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:B;CS251:C;CS213:C;CS210:B;CS259:D;MATH122:A;MATH241:A;MATH259:A;ENG101:A;ENG270:B;PSY102:B;HIS104:B;CHEM105:A;BIO121:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:A;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;HIS104:B;ECO102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:D;CS151:B;CS251:D;MATH122:A;MATH241:A;MATH259:A;ENG101:A;HIS104:B;PSY102:B;ECO102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:D;MATH122:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:B;CS151:A;CS251:C;CS213:A;CS210:A;CS259:B;CS451:C;CS462:B;CS281:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:B;ECO102:B;ENG270:B;PSY102:A;CHEM105:A;PHILOS100:C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:B;CS122:B;CS150:A;CS151:A;CS251:C;CS213:B;CS210:A;CS259:C;CS451:B;CS330:B;CS281:B;CS440:C;ML315:D;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:A;ENG270:A;PSY102:A;CHEM105:A;PHILOS100:A;BIO121:A;PSY211:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:B;CS151:B;CS251:A;CS213:D;CS210:A;CS259:B;MATH122:A;MATH241:A;MATH259:A;BIO121:B;PHY141:B;ENG101:A;ECO102:A;ENG270:A;CHEM105:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:A;CS151:A;CS251:B;CS213:B;CS210:B;CS259:C;CS451:C;CS330:D;CS317:B;CS440:C;CS281:A;MATH122:A;MATH241:A;MATH259:A;ENG101:A;ECE100:B;ECO102:A;ENG270:A;PSY102:A;CHEM105:A;BUSI100:B;BIO121:A;PSY211:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:B;CS251:C;CS213:B;CS210:A;CS259:B;CS451:D;CS462:D;CS281:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECO102:B;ENG270:A;PSY102:A;CHEM105:A;PHILOS100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:B;CS122:B;CS151:B;MATH122:A;MATH259:D;ENG101:D;CHEM105:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:A;CS151:A;CS251:B;CS213:B;CS210:A;CS259:B;CS451:A;CS330:A;CS281:A;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;CHEM105:A;ENG270:A;PSY102:A;BUSI100:A;PHILOS100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:B;CS251:B;CS213:D;CS210:D;CS259:B;MATH122:A;MATH241:B;MATH259:A;BIO121:A;HIS104:B;ENG101:A;ECO102:B;ECE100:A;PSY141:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:B;CS122:A;CS151:B;MATH122:A;MATH241:D;ENG101:A;PHY141:C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:B;CS151:A;CS251:A;CS213:A;CS210:A;CS259:A;CS451:A;CS317:A;CS281:A;CS330:A;HCI391:A;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;HIS104:A;ENG270:A;PSY102:A;CHEM105:A;PHILOS100:A;BIO121:A;PSY211:A;ECO102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:B;CS251:B;MATH122:A;MATH241:A;MATH259:A;ENG101:D;CHEM105:A;BIO121:A;ECO102:B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:B;CS151:A;CS251:B;MATH122:A;MATH241:D;MATH259:B;ENG101:A;CHEM105:A;BIO121:A;ECO102:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:B;CS151:A;CS251:A;CS213:C;CS210:A;CS259:C;CS451:B;CS281:A;CS462:B;CS330:A;SWE214:C;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECE100:B;ENG270:B;PSY102:A;CHEM105:B;PHILOS100:B;BIO121:A;HIS104:B;BUSI100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:A;CS150:B;CS151:B;CS251:A;CS213:B;CS210:B;CS259:C;CS451:B;CS317:A;CS281:B;MATH122:A;MATH241:A;MATH259:A;ENG101:A;PHY141:A;ECE100:A;HIS104:A;PSY102:A;PSY211:A;PHILOS100:A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS112:A;CS122:B;CS150:B;CS151:B;CS251:C;CS213:B;CS210:C;CS259:B;CS451:D;CS317:A;CS281:A;CS440:B;CS455:C;MATH122:A;MATH241:B;MATH259:A;ENG101:A;PHY141:A;ECO102:A;ECE100:A;PSY102:A;CHEM105:A;PHILOS100:A;ENG270:B;HIS104:B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -796,14 +824,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC693632-DE82-D54F-98DD-5166A338D32A}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="66" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.1640625" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="3" width="32.1640625" style="1"/>
-    <col min="4" max="4" width="216.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="32.1640625" style="1"/>
   </cols>
   <sheetData>
@@ -832,7 +860,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -840,13 +868,13 @@
         <v>20131177</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -854,13 +882,13 @@
         <v>20131184</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1">
@@ -868,13 +896,13 @@
         <v>20131208</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -883,13 +911,13 @@
         <v>20131407</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -898,13 +926,13 @@
         <v>20131477</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -913,13 +941,13 @@
         <v>20131582</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -928,13 +956,13 @@
         <v>20131603</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -943,13 +971,13 @@
         <v>20131753</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -958,13 +986,13 @@
         <v>20131767</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -973,13 +1001,13 @@
         <v>20131826</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -988,13 +1016,13 @@
         <v>20131850</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1003,13 +1031,13 @@
         <v>20131874</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1018,13 +1046,13 @@
         <v>20131889</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -1033,13 +1061,13 @@
         <v>20131936</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -1048,13 +1076,13 @@
         <v>20131998</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -1063,13 +1091,13 @@
         <v>20132032</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -1078,13 +1106,13 @@
         <v>20132136</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -1093,13 +1121,13 @@
         <v>20132137</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -1108,13 +1136,13 @@
         <v>20132193</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1123,13 +1151,13 @@
         <v>20132211</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -1138,13 +1166,13 @@
         <v>20132245</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -1153,13 +1181,13 @@
         <v>20132300</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -1168,13 +1196,13 @@
         <v>20132304</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -1183,13 +1211,13 @@
         <v>20132360</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1197,13 +1225,13 @@
         <v>20132369</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1211,13 +1239,13 @@
         <v>20132371</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="4" customFormat="1">
@@ -1225,13 +1253,13 @@
         <v>20132388</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1"/>
     </row>
@@ -1240,13 +1268,13 @@
         <v>20132422</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1255,13 +1283,13 @@
         <v>20132511</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E31" s="3"/>
     </row>
@@ -1270,13 +1298,13 @@
         <v>20132530</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E32" s="3"/>
     </row>
@@ -1285,13 +1313,13 @@
         <v>20132627</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1300,13 +1328,13 @@
         <v>20132654</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="E34" s="3"/>
     </row>
@@ -1315,13 +1343,13 @@
         <v>20132766</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E35" s="3"/>
     </row>
@@ -1330,13 +1358,13 @@
         <v>20132830</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E36" s="3"/>
     </row>
@@ -1345,13 +1373,13 @@
         <v>20132839</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1359,13 +1387,13 @@
         <v>20132852</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1373,13 +1401,13 @@
         <v>20132880</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1387,13 +1415,13 @@
         <v>20132884</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:5" customFormat="1">
@@ -1401,13 +1429,13 @@
         <v>20132911</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="E41" s="3"/>
     </row>
@@ -1416,13 +1444,13 @@
         <v>20132928</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1430,13 +1458,13 @@
         <v>20132939</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:5" customFormat="1">
@@ -1444,13 +1472,13 @@
         <v>20133005</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E44" s="3"/>
     </row>
@@ -1459,13 +1487,13 @@
         <v>20133050</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E45" s="3"/>
     </row>
@@ -1474,13 +1502,13 @@
         <v>20133095</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="E46" s="3"/>
     </row>
@@ -1489,13 +1517,13 @@
         <v>20133098</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E47" s="1"/>
     </row>
@@ -1504,13 +1532,13 @@
         <v>20133111</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E48" s="3"/>
     </row>
@@ -1519,13 +1547,13 @@
         <v>20133123</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1533,13 +1561,13 @@
         <v>20133184</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:5" customFormat="1">
@@ -1547,13 +1575,13 @@
         <v>20133211</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E51" s="3"/>
     </row>

</xml_diff>